<commit_message>
processed some statistics files
</commit_message>
<xml_diff>
--- a/EJBComponents/ImageProcessingBenchmark/stats/resourceContention/ExcelSheets/analysis-1-subImages.xlsx
+++ b/EJBComponents/ImageProcessingBenchmark/stats/resourceContention/ExcelSheets/analysis-1-subImages.xlsx
@@ -33,115 +33,115 @@
     <t>preparation</t>
   </si>
   <si>
-    <t>15:10:47 - 15:12:0</t>
-  </si>
-  <si>
     <t>grayscaling</t>
   </si>
   <si>
-    <t>15:12:0 - 15:13:42 (17.)</t>
-  </si>
-  <si>
     <t>errosion</t>
   </si>
   <si>
-    <t>15:15:3 - 15:16:32 (17.)</t>
-  </si>
-  <si>
     <t>image2</t>
   </si>
   <si>
-    <t>15:13:42 - 15:15:3</t>
-  </si>
-  <si>
-    <t>15:16:32 - 15:17:28 (17.)</t>
-  </si>
-  <si>
-    <t>15:18:47 - 15:21:18 (17.)</t>
-  </si>
-  <si>
     <t>image3</t>
   </si>
   <si>
-    <t>15:17:28 - 15:18:47</t>
-  </si>
-  <si>
-    <t>15:21:18 - 15:23:0 (17.)</t>
-  </si>
-  <si>
-    <t>15:27:23 - 15:28:59 (17.)</t>
-  </si>
-  <si>
     <t>image4</t>
   </si>
   <si>
-    <t>15:23:0 - 15:27:23</t>
-  </si>
-  <si>
-    <t>15:28:59 - 15:34:36 (17.)</t>
-  </si>
-  <si>
-    <t>15:41:34 - 15:46:49 (17.)</t>
-  </si>
-  <si>
     <t>image5</t>
   </si>
   <si>
-    <t>15:34:36 - 15:41:34</t>
-  </si>
-  <si>
-    <t>15:46:49 - 15:55:53 (17.)</t>
-  </si>
-  <si>
-    <t>15:55:53 - 16:4:20 (17.)</t>
-  </si>
-  <si>
     <t>1sub-images - time duration for each phase and the corresponding threads - RemoteOneNode</t>
   </si>
   <si>
-    <t>16:4:20 - 16:5:39</t>
-  </si>
-  <si>
-    <t>4:5:42 - 4:6:57 (101.)</t>
-  </si>
-  <si>
-    <t>4:6:58 - 4:6:59 (93.)</t>
-  </si>
-  <si>
-    <t>16:5:39 - 16:7:3</t>
-  </si>
-  <si>
-    <t>4:7:4 - 4:8:19 (101.)</t>
-  </si>
-  <si>
-    <t>4:8:21 - 4:8:22 (101.)</t>
-  </si>
-  <si>
-    <t>16:7:3 - 16:8:34</t>
-  </si>
-  <si>
-    <t>4:8:36 - 4:9:51 (110.)</t>
-  </si>
-  <si>
-    <t>4:9:53 - 4:9:53 (110.)</t>
-  </si>
-  <si>
-    <t>16:8:34 - 16:14:15</t>
-  </si>
-  <si>
-    <t>4:14:18 - 4:18:26 (107.)</t>
-  </si>
-  <si>
-    <t>4:18:29 - 4:18:31 (107.)</t>
-  </si>
-  <si>
-    <t>16:14:15 - 16:23:25</t>
-  </si>
-  <si>
-    <t>4:23:31 - 4:30:8 (86.)</t>
-  </si>
-  <si>
-    <t>4:30:14 - 4:30:16 (86.)</t>
+    <t>15:12:0 - 15:13:42 (17.) - (1:42) - (1:21)</t>
+  </si>
+  <si>
+    <t>15:15:3 - 15:16:32 (17.) - (1:29)</t>
+  </si>
+  <si>
+    <t>15:13:42 - 15:15:3 - (1:21) - (1:29)</t>
+  </si>
+  <si>
+    <t>15:16:32 - 15:17:28 (17.) - (0:56) - (1:19)</t>
+  </si>
+  <si>
+    <t>15:18:47 - 15:21:18 (17.) - (2:31)</t>
+  </si>
+  <si>
+    <t>15:17:28 - 15:18:47 - (1:19) - (2:31)</t>
+  </si>
+  <si>
+    <t>15:21:18 - 15:23:0 (17.) - (1:42) - (4:23)</t>
+  </si>
+  <si>
+    <t>15:27:23 - 15:28:59 (17.) - (1:36)</t>
+  </si>
+  <si>
+    <t>15:23:0 - 15:27:23 - (4:23) - (1:36)</t>
+  </si>
+  <si>
+    <t>15:28:59 - 15:34:36 (17.) - (5:37) - (6:58)</t>
+  </si>
+  <si>
+    <t>15:41:34 - 15:46:49 (17.) - (5:16)</t>
+  </si>
+  <si>
+    <t>15:34:36 - 15:41:34 - (6:58) - (5:16)</t>
+  </si>
+  <si>
+    <t>15:46:49 - 15:55:53 (17.) - (9:04) - (0)</t>
+  </si>
+  <si>
+    <t>15:55:53 - 16:4:20 (17.) - (8:27)</t>
+  </si>
+  <si>
+    <t>15:10:47 - 15:12:0 - (1:13) - (0)</t>
+  </si>
+  <si>
+    <t>16:4:20 - 16:5:39 - (1:19) - (0:3)</t>
+  </si>
+  <si>
+    <t>4:5:42 - 4:6:57 (101.) - (1:15) - (0:1)</t>
+  </si>
+  <si>
+    <t>4:6:58 - 4:6:59 (93.) - (0:1)</t>
+  </si>
+  <si>
+    <t>16:5:39 - 16:7:3 - (1:24) - (0:1)</t>
+  </si>
+  <si>
+    <t>4:7:4 - 4:8:19 (101.) - (1:15) - (0:2)</t>
+  </si>
+  <si>
+    <t>4:8:21 - 4:8:22 (101.) - (0:1)</t>
+  </si>
+  <si>
+    <t>16:7:3 - 16:8:34 - (1:31) - (0:2)</t>
+  </si>
+  <si>
+    <t>4:8:36 - 4:9:51 (110.) - (1:15) - (0:2)</t>
+  </si>
+  <si>
+    <t>4:9:53 - 4:9:53 (110.) - (0:0)</t>
+  </si>
+  <si>
+    <t>16:8:34 - 16:14:15 - (5:41) - (0:3)</t>
+  </si>
+  <si>
+    <t>4:14:18 - 4:18:26 (107.) - (0:8) - (0:3)</t>
+  </si>
+  <si>
+    <t>4:18:29 - 4:18:31 (107.) - (0:2)</t>
+  </si>
+  <si>
+    <t>16:14:15 - 16:23:25 - (9:10) - (0:6)</t>
+  </si>
+  <si>
+    <t>4:23:31 - 4:30:8 (86.) - (6:47) - (0:6)</t>
+  </si>
+  <si>
+    <t>4:30:14 - 4:30:16 (86.) - (0:2)</t>
   </si>
 </sst>
 </file>
@@ -639,10 +639,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:J32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,18 +979,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1005,28 +1005,28 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -1037,28 +1037,28 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -1069,28 +1069,28 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
@@ -1101,28 +1101,28 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
@@ -1138,7 +1138,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
@@ -1146,25 +1146,25 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
+      <c r="A32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -1184,7 +1184,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>27</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>28</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
         <v>31</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
         <v>2</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B47" t="s">
         <v>33</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
         <v>34</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
         <v>2</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" t="s">
         <v>36</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
         <v>37</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
         <v>2</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
         <v>39</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
         <v>40</v>

</xml_diff>